<commit_message>
Renamed CSV to Cluster.vi to xlsx to Cluster.vi, GUI updates to Main.vi, Documented Ballard Database Examples/Preliminary Ballard Database Template.xlsx and created Application/Installer build specs.
</commit_message>
<xml_diff>
--- a/Database Examples/Preliminary Ballard Database Template.xlsx
+++ b/Database Examples/Preliminary Ballard Database Template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkreienh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkreienh\Desktop\Ballard-Arinc-429-XML-Generator\Database Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D52D52-B33B-4B76-B32C-BEAE0323AE9C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B753809-430E-4DA8-85B1-A26579D2C2A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$9</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,8 +32,525 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jason Kreienheder</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AD869124-F1C1-4B2F-BB7E-097D8F4174C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ID:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the row ID and table length. "Row ID" can be used to re-sort the database. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6C8F17D1-7A07-4888-BA58-653F0F49BF8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Core Number:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the core number that gets appended to the filename of the generated Hardware and Parameter config files.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{61F720B4-6293-4EFA-842C-1CE2DA0134B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Channel Number:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the bus or channel as well as direction (Tx or Rx).
+For Rx use 0-15
+For Tx use 16-31</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{080E47FA-785A-4630-8607-38D9F9A9CC27}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Channel Name:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the bus or channel name. "Channel Name" values must be the same value when filtering by Core Number + Channel Number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{13710C80-205E-4C83-B3FC-02B502177A74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Channel Speed:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the Tx rate (12.5 or 100) of the bus or channel in KHz. "Channel Speed" values must be the same value when filtering by Core Number + Channel Number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{9C0C13C7-0A54-4BEF-A27F-117254E02EFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Label Octal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the octal label number (0-377)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{946E66AF-0234-4357-BFF1-9420B0D6CA43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Min Rate (mS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the minimum time in mS for the Tx scheduler. "Min Rate (mS)" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{9C4902DA-FC90-4386-813E-9CC53A4BA798}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Max Rate (mS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the maximum time in mS for the Tx scheduler. "Max Rate (mS)" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{B1F954A9-18C1-44B9-ABF9-471BB1C8486E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SDI:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the SDI value (0-4). "SDI" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{6CE513A5-BFC1-4C31-807B-554F17CE2B6E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SSM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the SSM value (0-4). "SSM" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{5A011551-F737-46D4-9FBF-D820F63975EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Create SDI:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies whether a SDI channel is created for the label. "Create SDI" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{1EAA3A08-0BC1-4296-89C8-528F43909F85}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Create SSM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies whether a SSM channel is created for the label. "Create SSM" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B6E18E54-1D4A-49AF-8112-749C331F7F1A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Create Parity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies whether a Parity channel is created for the label. "Create Parity" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{38D3B64B-BBB3-480B-A5D4-DF9FFEA0064E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parameter Name:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the Signal or Parameter Name. "Parameter Name" values must be unique when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{F5698B79-806B-495C-86BB-E8F83DA5DA62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Start Bit:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the start bit of the parameter (0-31) in the 32-bit word (zero index based).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{6C7F7423-029A-4EEB-99EC-E9EDB77277C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Number of Bits:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the length of the parameter (1-32) in the 32-bit word.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{CA849361-EA2D-451E-9F8E-3008190044E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Signal Type:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the signal type (scaled, uscaled, bcd or discrete) of the parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{FC6BFC64-DCAA-4A57-8F94-8F91F1480A77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Scale:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the scale applied to the parameter if the "Signal Type" is signed or usigned. If no value is specified, Scale will be set to 0.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{F7F1D8D3-9C26-48E3-8CA1-1776055A6014}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Offset:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the offset applied to the parameter if the "Signal Type" is signed or usigned. If no value is specified, Offset will be set to 0.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{158CE112-544C-43F0-8468-0068C6F24CD0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Units:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the engineering unit for Parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{51C632F4-ECE5-4F3E-A990-4728DDF4293B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Default Value:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specifies the default value for a Tx channel. If no value is specified, the default value will be set to 0.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>SDI</t>
   </si>
@@ -92,35 +609,51 @@
     <t>Create Parity</t>
   </si>
   <si>
-    <t>Singal Name</t>
-  </si>
-  <si>
     <t>LRU1</t>
   </si>
   <si>
-    <t>Minimum mS</t>
-  </si>
-  <si>
-    <t>Maximum mS</t>
-  </si>
-  <si>
     <t>Altitude_Rx</t>
   </si>
   <si>
     <t>LRU2</t>
+  </si>
+  <si>
+    <t>Min Rate (mS)</t>
+  </si>
+  <si>
+    <t>Max Rate (mS)</t>
+  </si>
+  <si>
+    <t>Parameter Name</t>
+  </si>
+  <si>
+    <t>Altitude_Tx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -465,36 +998,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DBCF9F-76BC-4534-AA02-79ECB42D2E30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DBCF9F-76BC-4534-AA02-79ECB42D2E30}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="70.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -517,10 +1049,10 @@
         <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
@@ -538,7 +1070,7 @@
         <v>18</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>2</v>
@@ -577,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>100</v>
@@ -607,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2">
         <v>25</v>
@@ -642,7 +1174,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
@@ -672,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O3" s="2">
         <v>25</v>
@@ -707,7 +1239,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
         <v>100</v>
@@ -737,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O4" s="2">
         <v>25</v>
@@ -766,7 +1298,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
@@ -796,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O5" s="2">
         <v>25</v>
@@ -825,7 +1357,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
@@ -855,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O6" s="2">
         <v>25</v>
@@ -886,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
         <v>100</v>
@@ -916,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O7" s="2">
         <v>25</v>
@@ -947,7 +1479,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
         <v>100</v>
@@ -977,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O8" s="2">
         <v>25</v>
@@ -1006,7 +1538,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2">
         <v>100</v>
@@ -1036,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O9" s="2">
         <v>25</v>
@@ -1055,7 +1587,31 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U3" xr:uid="{6A201D8D-5434-4FEC-B280-B22C4DA13095}"/>
+  <autoFilter ref="A1:U9" xr:uid="{6A201D8D-5434-4FEC-B280-B22C4DA13095}"/>
+  <dataValidations count="6">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are 12.5 and 100 kHz" promptTitle="Alert" prompt="message here" sqref="E2:E1048576" xr:uid="{5C2CF8C6-1084-447E-93BA-5AE18D9D43C2}">
+      <formula1>"12.5,100"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are 0-31" sqref="C2:C1048576 O2:O1048576" xr:uid="{DFAEAB8C-C211-4454-828F-5CC9DDC4C4C9}">
+      <formula1>0</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are 0-377" sqref="F2:F1048576" xr:uid="{1B4A023E-DDA2-40D6-940E-97F21F57B76D}">
+      <formula1>0</formula1>
+      <formula2>377</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are TRUE or FALSE" sqref="K2:M1048576" xr:uid="{C876F880-4E40-40F4-B9DE-95F6096DB3B2}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are 1-32" sqref="P2:P1048576" xr:uid="{72C81608-E19A-4C1B-87E6-77611AB52CB2}">
+      <formula1>1</formula1>
+      <formula2>32</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are scaled, uscaled, discrete or bcd." sqref="Q2:Q1048576" xr:uid="{E0DF19B2-72C2-4144-9627-354390583FC0}">
+      <formula1>"scaled,uscaled,bcd,discrete"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Main.vi and Check Database For Entry Errors.vi to prevent configuration files from being created upon error. Fixes #2. Minor updates to Preliminary Ballard Database Template.xlsx to document "Default Value".
</commit_message>
<xml_diff>
--- a/Database Examples/Preliminary Ballard Database Template.xlsx
+++ b/Database Examples/Preliminary Ballard Database Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkreienh\Desktop\Ballard-Arinc-429-XML-Generator\Database Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B753809-430E-4DA8-85B1-A26579D2C2A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1BF73-0AA0-43C9-BC7D-EB0A15CAF14C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$9</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -253,7 +253,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Specifies the SDI value (0-4). "SDI" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+Specifies the SDI value (0-4). "SDI" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI
+0 - SDI = "00"
+1 - SDI = "01"
+2 - SDI = "10"
+3 - SDI = "11"
+4 - SDI = "All" for Tx and "Off" for Rx</t>
         </r>
       </text>
     </comment>
@@ -277,7 +282,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Specifies the SSM value (0-4). "SSM" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI</t>
+Specifies the SSM value (0-4). "SSM" values must be the same value when filtering by Core Number + Channel Number + Label Octal + SDI
+0 - SSM = "00"
+1 - SSM = "01"
+2 - SSM = "10"
+3 - SSM = "11"
+4 - SSM = "?"</t>
         </r>
       </text>
     </comment>
@@ -435,7 +445,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Signal Type:</t>
+          <t>Parameter Type:</t>
         </r>
         <r>
           <rPr>
@@ -541,7 +551,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Specifies the default value for a Tx channel. If no value is specified, the default value will be set to 0.</t>
+Specifies the scaled Parameter's default value for a Tx channel. If no value is specified, the default value will be set to 0.</t>
         </r>
       </text>
     </comment>
@@ -561,9 +571,6 @@
     <t>Start Bit</t>
   </si>
   <si>
-    <t>Signal Type</t>
-  </si>
-  <si>
     <t>Offset</t>
   </si>
   <si>
@@ -628,6 +635,9 @@
   </si>
   <si>
     <t>Altitude_Tx</t>
+  </si>
+  <si>
+    <t>Parameter Type</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1012,7 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1032,7 @@
     <col min="14" max="14" width="21.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.21875" style="1" bestFit="1" customWidth="1"/>
@@ -1031,67 +1041,67 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
@@ -1109,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2">
         <v>100</v>
@@ -1139,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O2" s="2">
         <v>25</v>
@@ -1148,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -1174,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
@@ -1204,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" s="2">
         <v>25</v>
@@ -1213,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -1239,7 +1249,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2">
         <v>100</v>
@@ -1269,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" s="2">
         <v>25</v>
@@ -1278,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -1298,7 +1308,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
@@ -1328,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O5" s="2">
         <v>25</v>
@@ -1337,7 +1347,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -1357,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
@@ -1387,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="2">
         <v>25</v>
@@ -1396,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -1418,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>100</v>
@@ -1448,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2">
         <v>25</v>
@@ -1457,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R7" s="2">
         <v>1</v>
@@ -1479,7 +1489,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
         <v>100</v>
@@ -1509,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O8" s="2">
         <v>25</v>
@@ -1518,7 +1528,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R8" s="2">
         <v>1</v>
@@ -1538,7 +1548,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
         <v>100</v>
@@ -1568,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O9" s="2">
         <v>25</v>
@@ -1577,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R9" s="2">
         <v>1</v>
@@ -1587,7 +1597,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U9" xr:uid="{6A201D8D-5434-4FEC-B280-B22C4DA13095}"/>
+  <autoFilter ref="A1:Y9" xr:uid="{75341374-CB54-49B7-84BF-9FDDAD8C028E}"/>
   <dataValidations count="6">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" errorTitle="Alert" error="Valid Entries are 12.5 and 100 kHz" promptTitle="Alert" prompt="message here" sqref="E2:E1048576" xr:uid="{5C2CF8C6-1084-447E-93BA-5AE18D9D43C2}">
       <formula1>"12.5,100"</formula1>

</xml_diff>